<commit_message>
added python 2.7 script
</commit_message>
<xml_diff>
--- a/allPDF.xlsx
+++ b/allPDF.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etienne\Documents\GitHub\From-PDF-to-Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17865" windowHeight="7395"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Total Revenue</t>
   </si>
@@ -67,39 +63,151 @@
   </si>
   <si>
     <t>Earnings Per Share (EPS)</t>
+  </si>
+  <si>
+    <t>100000.00</t>
+  </si>
+  <si>
+    <t>-20000.00</t>
+  </si>
+  <si>
+    <t>80000.00</t>
+  </si>
+  <si>
+    <t>-30000.00</t>
+  </si>
+  <si>
+    <t>10000.00</t>
+  </si>
+  <si>
+    <t>5000.00</t>
+  </si>
+  <si>
+    <t>50000.00</t>
+  </si>
+  <si>
+    <t>-10000.00</t>
+  </si>
+  <si>
+    <t>40000.00</t>
+  </si>
+  <si>
+    <t>30000.00</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>179655.00</t>
+  </si>
+  <si>
+    <t>-365600.00</t>
+  </si>
+  <si>
+    <t>193263.00</t>
+  </si>
+  <si>
+    <t>-157091.00</t>
+  </si>
+  <si>
+    <t>495803.00</t>
+  </si>
+  <si>
+    <t>146622.00</t>
+  </si>
+  <si>
+    <t>100819.00</t>
+  </si>
+  <si>
+    <t>471764.00</t>
+  </si>
+  <si>
+    <t>251942.00</t>
+  </si>
+  <si>
+    <t>-352836.00</t>
+  </si>
+  <si>
+    <t>408964.00</t>
+  </si>
+  <si>
+    <t>-94366.00</t>
+  </si>
+  <si>
+    <t>393698.00</t>
+  </si>
+  <si>
+    <t>187967.00</t>
+  </si>
+  <si>
+    <t>1860604.00</t>
+  </si>
+  <si>
+    <t>364466.00</t>
+  </si>
+  <si>
+    <t>-266995.00</t>
+  </si>
+  <si>
+    <t>40632.00</t>
+  </si>
+  <si>
+    <t>-236492.00</t>
+  </si>
+  <si>
+    <t>102830.00</t>
+  </si>
+  <si>
+    <t>362878.00</t>
+  </si>
+  <si>
+    <t>383220.00</t>
+  </si>
+  <si>
+    <t>291758.00</t>
+  </si>
+  <si>
+    <t>214391.00</t>
+  </si>
+  <si>
+    <t>-403289.00</t>
+  </si>
+  <si>
+    <t>326556.00</t>
+  </si>
+  <si>
+    <t>-137757.00</t>
+  </si>
+  <si>
+    <t>376483.00</t>
+  </si>
+  <si>
+    <t>450211.00</t>
+  </si>
+  <si>
+    <t>1868892.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -114,47 +222,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -442,21 +529,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="15" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,157 +592,157 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>100000</v>
-      </c>
-      <c r="B2" s="3">
-        <v>-20000</v>
-      </c>
-      <c r="C2" s="3">
-        <v>80000</v>
-      </c>
-      <c r="D2" s="3">
-        <v>-30000</v>
-      </c>
-      <c r="E2" s="3">
-        <v>10000</v>
-      </c>
-      <c r="F2" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G2" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H2" s="3">
-        <v>5000</v>
-      </c>
-      <c r="I2" s="3">
-        <v>-30000</v>
-      </c>
-      <c r="J2" s="3">
-        <v>50000</v>
-      </c>
-      <c r="K2" s="3">
-        <v>-10000</v>
-      </c>
-      <c r="L2" s="3">
-        <v>40000</v>
-      </c>
-      <c r="M2" s="3">
-        <v>-10000</v>
-      </c>
-      <c r="N2" s="3">
-        <v>30000</v>
-      </c>
-      <c r="O2" s="3">
-        <v>30000</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1</v>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>179655</v>
-      </c>
-      <c r="B3" s="3">
-        <v>-365600</v>
-      </c>
-      <c r="C3" s="3">
-        <v>193263</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-157091</v>
-      </c>
-      <c r="E3" s="3">
-        <v>495803</v>
-      </c>
-      <c r="F3" s="3">
-        <v>146622</v>
-      </c>
-      <c r="G3" s="3">
-        <v>100819</v>
-      </c>
-      <c r="H3" s="3">
-        <v>471764</v>
-      </c>
-      <c r="I3" s="3">
-        <v>-157091</v>
-      </c>
-      <c r="J3" s="3">
-        <v>251942</v>
-      </c>
-      <c r="K3" s="3">
-        <v>-352836</v>
-      </c>
-      <c r="L3" s="3">
-        <v>408964</v>
-      </c>
-      <c r="M3" s="3">
-        <v>-94366</v>
-      </c>
-      <c r="N3" s="3">
-        <v>393698</v>
-      </c>
-      <c r="O3" s="3">
-        <v>187967</v>
-      </c>
-      <c r="P3" s="3">
-        <v>1860604</v>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>364466</v>
-      </c>
-      <c r="B4" s="3">
-        <v>-266995</v>
-      </c>
-      <c r="C4" s="3">
-        <v>40632</v>
-      </c>
-      <c r="D4" s="3">
-        <v>-236492</v>
-      </c>
-      <c r="E4" s="3">
-        <v>102830</v>
-      </c>
-      <c r="F4" s="3">
-        <v>362878</v>
-      </c>
-      <c r="G4" s="3">
-        <v>383220</v>
-      </c>
-      <c r="H4" s="3">
-        <v>291758</v>
-      </c>
-      <c r="I4" s="3">
-        <v>-236492</v>
-      </c>
-      <c r="J4" s="3">
-        <v>214391</v>
-      </c>
-      <c r="K4" s="3">
-        <v>-403289</v>
-      </c>
-      <c r="L4" s="3">
-        <v>326556</v>
-      </c>
-      <c r="M4" s="3">
-        <v>-137757</v>
-      </c>
-      <c r="N4" s="3">
-        <v>376483</v>
-      </c>
-      <c r="O4" s="3">
-        <v>450211</v>
-      </c>
-      <c r="P4" s="3">
-        <v>1868892</v>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>